<commit_message>
swapped 0.2uF for 0.1uF, updated BoM
</commit_message>
<xml_diff>
--- a/Electronics/Low Level v3/BoM.xlsx
+++ b/Electronics/Low Level v3/BoM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Projects/elcano/Electronics/Low Level v3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EE2B06-6A63-1A45-AEBA-31524264614F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8040C5-3CD6-5A4E-9A8B-F0569C8CC28A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="20560" xr2:uid="{F66CC82F-6637-7D48-A4BB-0FCD493187ED}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="LowLevelv3" localSheetId="0">Sheet1!$A$1:$X$31</definedName>
+    <definedName name="LowLevelv3" localSheetId="0">Sheet1!$A$1:$X$29</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="197">
   <si>
     <t>Qty</t>
   </si>
@@ -209,12 +209,6 @@
     <t>CAPACITOR, American symbol</t>
   </si>
   <si>
-    <t>1 uF</t>
-  </si>
-  <si>
-    <t>C9</t>
-  </si>
-  <si>
     <t>R-US_R1206</t>
   </si>
   <si>
@@ -299,15 +293,6 @@
     <t>1uF</t>
   </si>
   <si>
-    <t>C1, C2, C3, C4</t>
-  </si>
-  <si>
-    <t>200nF</t>
-  </si>
-  <si>
-    <t>C15, C16</t>
-  </si>
-  <si>
     <t>20K</t>
   </si>
   <si>
@@ -645,6 +630,33 @@
   </si>
   <si>
     <t>Part Label</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C4, C9, C15, C16</t>
+  </si>
+  <si>
+    <t>732-7873-1-ND</t>
+  </si>
+  <si>
+    <t>RMCF1206JT10K0CT-ND</t>
+  </si>
+  <si>
+    <t>311-100FRCT-ND</t>
+  </si>
+  <si>
+    <t>A129547CT-ND</t>
+  </si>
+  <si>
+    <t>RNCP1206FTD1K00CT-ND</t>
+  </si>
+  <si>
+    <t>RNCP1206FTD20K0CT-ND</t>
+  </si>
+  <si>
+    <t>A106078CT-ND</t>
+  </si>
+  <si>
+    <t>311-4436-1-ND</t>
   </si>
 </sst>
 </file>
@@ -703,12 +715,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -717,6 +726,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1036,18 +1051,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A12E2CF-710F-D148-A35C-437BFC6C6DF7}">
-  <dimension ref="A1:W40"/>
+  <dimension ref="A1:W38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="141" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.1640625" customWidth="1"/>
-    <col min="3" max="3" width="35.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" style="6" customWidth="1"/>
     <col min="5" max="5" width="18.5" customWidth="1"/>
     <col min="6" max="6" width="31.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.83203125" bestFit="1" customWidth="1"/>
@@ -1073,22 +1088,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>165</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>
@@ -1144,13 +1159,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
-      </c>
-      <c r="D2" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>184</v>
       </c>
       <c r="F2" t="s">
         <v>25</v>
@@ -1164,25 +1179,25 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>190</v>
+      <c r="C3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>189</v>
       </c>
       <c r="F3" t="s">
         <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="H3" t="s">
         <v>46</v>
@@ -1190,25 +1205,25 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>191</v>
+      <c r="C4" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>196</v>
       </c>
       <c r="F4" t="s">
         <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="H4" t="s">
         <v>46</v>
@@ -1216,19 +1231,25 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>76</v>
+      <c r="C5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>185</v>
       </c>
       <c r="F5" t="s">
         <v>44</v>
       </c>
       <c r="G5" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="H5" t="s">
         <v>46</v>
@@ -1236,19 +1257,25 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>78</v>
+      <c r="C6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>186</v>
       </c>
       <c r="F6" t="s">
         <v>44</v>
       </c>
       <c r="G6" t="s">
-        <v>79</v>
+        <v>188</v>
       </c>
       <c r="H6" t="s">
         <v>46</v>
@@ -1259,99 +1286,129 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="4">
+        <v>100</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="F7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="5">
-        <v>100</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>50</v>
-      </c>
-      <c r="G7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H7" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>195</v>
       </c>
       <c r="F8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H8" t="s">
         <v>50</v>
-      </c>
-      <c r="G8" t="s">
-        <v>54</v>
-      </c>
-      <c r="H8" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="5">
-        <v>120</v>
+        <v>47</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>190</v>
       </c>
       <c r="F9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" t="s">
         <v>50</v>
-      </c>
-      <c r="G9" t="s">
-        <v>55</v>
-      </c>
-      <c r="H9" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>67</v>
+        <v>47</v>
+      </c>
+      <c r="C10" s="4">
+        <v>120</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>192</v>
       </c>
       <c r="F10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" t="s">
         <v>50</v>
-      </c>
-      <c r="G10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H10" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>80</v>
+        <v>47</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>193</v>
       </c>
       <c r="F11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" t="s">
         <v>50</v>
-      </c>
-      <c r="G11" t="s">
-        <v>81</v>
-      </c>
-      <c r="H11" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
@@ -1359,98 +1416,98 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>181</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E12" t="s">
-        <v>62</v>
+        <v>47</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>194</v>
       </c>
       <c r="F12" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="G12" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="H12" t="s">
-        <v>60</v>
-      </c>
-      <c r="I12" t="s">
-        <v>61</v>
-      </c>
-      <c r="J12" t="s">
-        <v>62</v>
-      </c>
-      <c r="K12" t="s">
-        <v>63</v>
-      </c>
-      <c r="M12" t="s">
-        <v>64</v>
-      </c>
-      <c r="N12" t="s">
-        <v>57</v>
-      </c>
-      <c r="R12" t="s">
-        <v>65</v>
-      </c>
-      <c r="U12" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>183</v>
+        <v>176</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E13" t="s">
+        <v>60</v>
       </c>
       <c r="F13" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="G13" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="H13" t="s">
-        <v>72</v>
+        <v>58</v>
+      </c>
+      <c r="I13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J13" t="s">
+        <v>60</v>
+      </c>
+      <c r="K13" t="s">
+        <v>61</v>
+      </c>
+      <c r="M13" t="s">
+        <v>62</v>
+      </c>
+      <c r="N13" t="s">
+        <v>55</v>
+      </c>
+      <c r="R13" t="s">
+        <v>63</v>
+      </c>
+      <c r="U13" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>186</v>
+        <v>67</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>178</v>
       </c>
       <c r="F14" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G14" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
@@ -1458,54 +1515,54 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>182</v>
+        <v>71</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>181</v>
       </c>
       <c r="F15" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="G15" t="s">
-        <v>83</v>
-      </c>
-      <c r="L15">
-        <v>2845124</v>
-      </c>
-      <c r="W15" t="s">
-        <v>84</v>
+        <v>73</v>
+      </c>
+      <c r="H15" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>187</v>
+        <v>77</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>177</v>
       </c>
       <c r="F16" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G16" t="s">
-        <v>87</v>
-      </c>
-      <c r="H16" t="s">
-        <v>88</v>
+        <v>78</v>
+      </c>
+      <c r="L16">
+        <v>2845124</v>
+      </c>
+      <c r="W16" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
@@ -1513,39 +1570,57 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>89</v>
+        <v>80</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>182</v>
       </c>
       <c r="F17" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="G17" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="H17" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>91</v>
+        <v>99</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="F18" t="s">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G18" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="H18" t="s">
-        <v>52</v>
+        <v>102</v>
+      </c>
+      <c r="S18" t="s">
+        <v>103</v>
+      </c>
+      <c r="T18" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
@@ -1553,19 +1628,43 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>96</v>
+        <v>149</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E19" t="s">
+        <v>154</v>
       </c>
       <c r="F19" t="s">
-        <v>44</v>
+        <v>150</v>
       </c>
       <c r="G19" t="s">
-        <v>97</v>
+        <v>151</v>
       </c>
       <c r="H19" t="s">
-        <v>46</v>
+        <v>152</v>
+      </c>
+      <c r="I19" t="s">
+        <v>153</v>
+      </c>
+      <c r="J19" t="s">
+        <v>154</v>
+      </c>
+      <c r="K19" t="s">
+        <v>155</v>
+      </c>
+      <c r="M19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N19" t="s">
+        <v>149</v>
+      </c>
+      <c r="R19" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
@@ -1573,74 +1672,44 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>104</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>189</v>
+        <v>106</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="F20" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G20" t="s">
-        <v>106</v>
-      </c>
-      <c r="H20" t="s">
         <v>107</v>
-      </c>
-      <c r="S20" t="s">
-        <v>108</v>
-      </c>
-      <c r="T20" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>154</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>171</v>
+        <v>158</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>166</v>
       </c>
       <c r="E21" t="s">
+        <v>167</v>
+      </c>
+      <c r="F21" t="s">
         <v>159</v>
       </c>
-      <c r="F21" t="s">
-        <v>155</v>
-      </c>
       <c r="G21" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="H21" t="s">
-        <v>157</v>
-      </c>
-      <c r="I21" t="s">
-        <v>158</v>
-      </c>
-      <c r="J21" t="s">
-        <v>159</v>
-      </c>
-      <c r="K21" t="s">
-        <v>160</v>
-      </c>
-      <c r="M21" t="s">
         <v>161</v>
       </c>
-      <c r="N21" t="s">
-        <v>154</v>
-      </c>
-      <c r="R21" t="s">
+      <c r="U21" t="s">
         <v>162</v>
       </c>
     </row>
@@ -1649,16 +1718,34 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>111</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>110</v>
+        <v>36</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>175</v>
       </c>
       <c r="F22" t="s">
-        <v>111</v>
+        <v>37</v>
       </c>
       <c r="G22" t="s">
-        <v>112</v>
+        <v>38</v>
+      </c>
+      <c r="H22" t="s">
+        <v>39</v>
+      </c>
+      <c r="S22" t="s">
+        <v>40</v>
+      </c>
+      <c r="U22" t="s">
+        <v>41</v>
+      </c>
+      <c r="V22" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
@@ -1666,28 +1753,28 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>163</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E23" t="s">
-        <v>172</v>
+        <v>129</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="F23" t="s">
-        <v>164</v>
+        <v>130</v>
       </c>
       <c r="G23" t="s">
-        <v>165</v>
+        <v>131</v>
       </c>
       <c r="H23" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
       <c r="U23" t="s">
-        <v>167</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
@@ -1695,34 +1782,25 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>180</v>
+        <v>134</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="F24" t="s">
-        <v>37</v>
+        <v>135</v>
       </c>
       <c r="G24" t="s">
-        <v>38</v>
+        <v>136</v>
       </c>
       <c r="H24" t="s">
-        <v>39</v>
-      </c>
-      <c r="S24" t="s">
-        <v>40</v>
-      </c>
-      <c r="U24" t="s">
-        <v>41</v>
-      </c>
-      <c r="V24" t="s">
-        <v>35</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
@@ -1730,28 +1808,31 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>134</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D25" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>178</v>
-      </c>
       <c r="F25" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="G25" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="H25" t="s">
-        <v>137</v>
-      </c>
-      <c r="U25" t="s">
-        <v>41</v>
+        <v>141</v>
+      </c>
+      <c r="S25" t="s">
+        <v>142</v>
+      </c>
+      <c r="T25" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
@@ -1759,25 +1840,22 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>139</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>177</v>
+        <v>19</v>
       </c>
       <c r="F26" t="s">
-        <v>140</v>
+        <v>20</v>
       </c>
       <c r="G26" t="s">
-        <v>141</v>
+        <v>21</v>
       </c>
       <c r="H26" t="s">
-        <v>142</v>
+        <v>22</v>
+      </c>
+      <c r="S26" t="s">
+        <v>23</v>
+      </c>
+      <c r="T26" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
@@ -1785,31 +1863,28 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>143</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>176</v>
+        <v>88</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="F27" t="s">
-        <v>144</v>
+        <v>89</v>
       </c>
       <c r="G27" t="s">
-        <v>145</v>
-      </c>
-      <c r="H27" t="s">
-        <v>146</v>
-      </c>
-      <c r="S27" t="s">
-        <v>147</v>
-      </c>
-      <c r="T27" t="s">
-        <v>148</v>
+        <v>90</v>
+      </c>
+      <c r="L27">
+        <v>51040694</v>
+      </c>
+      <c r="W27" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
@@ -1817,22 +1892,31 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>19</v>
+        <v>109</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="F28" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="G28" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
       <c r="H28" t="s">
-        <v>22</v>
+        <v>112</v>
       </c>
       <c r="S28" t="s">
-        <v>23</v>
-      </c>
-      <c r="T28" t="s">
-        <v>24</v>
+        <v>113</v>
+      </c>
+      <c r="U28" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
@@ -1840,28 +1924,31 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>93</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>188</v>
+        <v>144</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="F29" t="s">
-        <v>94</v>
+        <v>145</v>
       </c>
       <c r="G29" t="s">
-        <v>95</v>
-      </c>
-      <c r="L29">
-        <v>51040694</v>
-      </c>
-      <c r="W29" t="s">
-        <v>84</v>
+        <v>146</v>
+      </c>
+      <c r="H29" t="s">
+        <v>147</v>
+      </c>
+      <c r="P29" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
@@ -1869,31 +1956,16 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>114</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>175</v>
+        <v>28</v>
       </c>
       <c r="F30" t="s">
-        <v>115</v>
+        <v>29</v>
       </c>
       <c r="G30" t="s">
-        <v>116</v>
+        <v>30</v>
       </c>
       <c r="H30" t="s">
-        <v>117</v>
-      </c>
-      <c r="S30" t="s">
-        <v>118</v>
-      </c>
-      <c r="U30" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
@@ -1901,31 +1973,16 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>149</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>174</v>
+        <v>32</v>
       </c>
       <c r="F31" t="s">
-        <v>150</v>
+        <v>33</v>
       </c>
       <c r="G31" t="s">
-        <v>151</v>
+        <v>34</v>
       </c>
       <c r="H31" t="s">
-        <v>152</v>
-      </c>
-      <c r="P31" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>153</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
@@ -1933,13 +1990,16 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>127</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="F32" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="G32" t="s">
-        <v>30</v>
+        <v>126</v>
       </c>
       <c r="H32" t="s">
         <v>31</v>
@@ -1950,13 +2010,16 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>94</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="F33" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="G33" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="H33" t="s">
         <v>31</v>
@@ -1967,16 +2030,16 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>132</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>131</v>
+        <v>94</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="F34" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="G34" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="H34" t="s">
         <v>31</v>
@@ -1987,16 +2050,16 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>99</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>119</v>
+        <v>94</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="F35" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G35" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="H35" t="s">
         <v>31</v>
@@ -2007,16 +2070,16 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>99</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>121</v>
+        <v>94</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="F36" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G36" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="H36" t="s">
         <v>31</v>
@@ -2027,16 +2090,16 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>99</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>98</v>
+        <v>119</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>118</v>
       </c>
       <c r="F37" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="G37" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="H37" t="s">
         <v>31</v>
@@ -2047,66 +2110,35 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>99</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>102</v>
+        <v>123</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="F38" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="G38" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="H38" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>1</v>
-      </c>
-      <c r="B39" t="s">
-        <v>124</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="F39" t="s">
-        <v>125</v>
-      </c>
-      <c r="G39" t="s">
-        <v>126</v>
-      </c>
-      <c r="H39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>1</v>
-      </c>
-      <c r="B40" t="s">
-        <v>128</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="F40" t="s">
-        <v>129</v>
-      </c>
-      <c r="G40" t="s">
-        <v>130</v>
-      </c>
-      <c r="H40" t="s">
-        <v>31</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/885012208009/732-8086-1-ND/5454713" xr:uid="{D80452D3-1A69-A54A-A661-98A1D5AE806B}"/>
-    <hyperlink ref="E4" r:id="rId2" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/885012208013/732-7685-1-ND/5454312" xr:uid="{D9F1E12D-E34B-E84B-8B4B-EFA495912CD3}"/>
+    <hyperlink ref="E5" r:id="rId1" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/885012208009/732-8086-1-ND/5454713" xr:uid="{D80452D3-1A69-A54A-A661-98A1D5AE806B}"/>
+    <hyperlink ref="E6" r:id="rId2" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/885012208013/732-7685-1-ND/5454312" xr:uid="{D9F1E12D-E34B-E84B-8B4B-EFA495912CD3}"/>
+    <hyperlink ref="E3" r:id="rId3" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/885012008020/732-7873-1-ND/5454500" xr:uid="{4684C06F-18A2-F04E-9C05-4F3BEFCCB8D6}"/>
+    <hyperlink ref="E9" r:id="rId4" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RMCF1206JT10K0/RMCF1206JT10K0CT-ND/1942803" xr:uid="{C8C79A7E-5B0A-E74A-BA35-E9B6228D05E3}"/>
+    <hyperlink ref="E7" r:id="rId5" display="https://www.digikey.com/product-detail/en/yageo/RC1206FR-07100RL/311-100FRCT-ND/731438" xr:uid="{1C9816EA-FD83-1441-B8D7-C0EE52E11431}"/>
+    <hyperlink ref="E10" r:id="rId6" display="https://www.digikey.com/product-detail/en/te-connectivity-passive-product/CRGH1206F120R/A129547CT-ND/8566751" xr:uid="{C6DA220A-4451-814A-9E55-AA6029F5FAB9}"/>
+    <hyperlink ref="E11" r:id="rId7" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP1206FTD1K00/RNCP1206FTD1K00CT-ND/2240675" xr:uid="{87925A96-0F2A-0D47-9995-734FF133B0B8}"/>
+    <hyperlink ref="E12" r:id="rId8" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP1206FTD20K0/RNCP1206FTD20K0CT-ND/2240718" xr:uid="{116631FA-D811-884C-B276-9CADAAEF69F4}"/>
+    <hyperlink ref="E8" r:id="rId9" display="https://www.digikey.com/product-detail/en/te-connectivity-passive-product/CRG1206F4K7/A106078CT-ND/3477735" xr:uid="{54F5A1F9-1D87-0A40-A492-AFC72B5AAEE0}"/>
+    <hyperlink ref="E4" r:id="rId10" display="https://www.digikey.com/product-detail/en/yageo/CC1206JRNPOBBN561/311-4436-1-ND/8025525" xr:uid="{39858258-CC5F-A247-B310-151D6A733093}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added screw terminal to BoM
</commit_message>
<xml_diff>
--- a/Electronics/Low Level v3/BoM.xlsx
+++ b/Electronics/Low Level v3/BoM.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Projects/elcano/Electronics/Low Level v3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8040C5-3CD6-5A4E-9A8B-F0569C8CC28A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B53FC5D-3B06-A245-ADBA-15DAD99665E4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="20560" xr2:uid="{F66CC82F-6637-7D48-A4BB-0FCD493187ED}"/>
+    <workbookView xWindow="0" yWindow="1040" windowWidth="33600" windowHeight="20560" xr2:uid="{F66CC82F-6637-7D48-A4BB-0FCD493187ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="LowLevelv3" localSheetId="0">Sheet1!$A$1:$X$29</definedName>
+    <definedName name="LowLevelv3" localSheetId="0">Sheet1!$A$1:$X$28</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="198">
   <si>
     <t>Qty</t>
   </si>
@@ -657,6 +657,9 @@
   </si>
   <si>
     <t>311-4436-1-ND</t>
+  </si>
+  <si>
+    <t>732-2031-ND</t>
   </si>
 </sst>
 </file>
@@ -1051,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A12E2CF-710F-D148-A35C-437BFC6C6DF7}">
-  <dimension ref="A1:W38"/>
+  <dimension ref="A1:W39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1672,16 +1675,28 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>106</v>
+        <v>158</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>105</v>
+        <v>158</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E20" t="s">
+        <v>167</v>
       </c>
       <c r="F20" t="s">
-        <v>106</v>
+        <v>159</v>
       </c>
       <c r="G20" t="s">
-        <v>107</v>
+        <v>160</v>
+      </c>
+      <c r="H20" t="s">
+        <v>161</v>
+      </c>
+      <c r="U20" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
@@ -1689,28 +1704,34 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>158</v>
+        <v>36</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>158</v>
+        <v>35</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="E21" t="s">
-        <v>167</v>
+        <v>174</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>175</v>
       </c>
       <c r="F21" t="s">
-        <v>159</v>
+        <v>37</v>
       </c>
       <c r="G21" t="s">
-        <v>160</v>
+        <v>38</v>
       </c>
       <c r="H21" t="s">
-        <v>161</v>
+        <v>39</v>
+      </c>
+      <c r="S21" t="s">
+        <v>40</v>
       </c>
       <c r="U21" t="s">
-        <v>162</v>
+        <v>41</v>
+      </c>
+      <c r="V21" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
@@ -1718,63 +1739,54 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>129</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>35</v>
+        <v>129</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F22" t="s">
-        <v>37</v>
+        <v>130</v>
       </c>
       <c r="G22" t="s">
-        <v>38</v>
+        <v>131</v>
       </c>
       <c r="H22" t="s">
-        <v>39</v>
-      </c>
-      <c r="S22" t="s">
-        <v>40</v>
+        <v>132</v>
       </c>
       <c r="U22" t="s">
         <v>41</v>
       </c>
-      <c r="V22" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>166</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F23" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="G23" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="H23" t="s">
-        <v>132</v>
-      </c>
-      <c r="U23" t="s">
-        <v>41</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
@@ -1782,25 +1794,31 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>166</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F24" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="G24" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="H24" t="s">
-        <v>137</v>
+        <v>141</v>
+      </c>
+      <c r="S24" t="s">
+        <v>142</v>
+      </c>
+      <c r="T24" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
@@ -1808,31 +1826,28 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>138</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>138</v>
+        <v>19</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>171</v>
+        <v>174</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>197</v>
       </c>
       <c r="F25" t="s">
-        <v>139</v>
+        <v>20</v>
       </c>
       <c r="G25" t="s">
-        <v>140</v>
+        <v>21</v>
       </c>
       <c r="H25" t="s">
-        <v>141</v>
+        <v>22</v>
       </c>
       <c r="S25" t="s">
-        <v>142</v>
+        <v>23</v>
       </c>
       <c r="T25" t="s">
-        <v>143</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
@@ -1840,22 +1855,28 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>88</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="F26" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="G26" t="s">
-        <v>21</v>
-      </c>
-      <c r="H26" t="s">
-        <v>22</v>
-      </c>
-      <c r="S26" t="s">
-        <v>23</v>
-      </c>
-      <c r="T26" t="s">
-        <v>24</v>
+        <v>90</v>
+      </c>
+      <c r="L26">
+        <v>51040694</v>
+      </c>
+      <c r="W26" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
@@ -1863,28 +1884,31 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="F27" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="G27" t="s">
-        <v>90</v>
-      </c>
-      <c r="L27">
-        <v>51040694</v>
-      </c>
-      <c r="W27" t="s">
-        <v>79</v>
+        <v>111</v>
+      </c>
+      <c r="H27" t="s">
+        <v>112</v>
+      </c>
+      <c r="S27" t="s">
+        <v>113</v>
+      </c>
+      <c r="U27" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
@@ -1892,31 +1916,31 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>108</v>
+        <v>168</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>166</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F28" t="s">
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="G28" t="s">
-        <v>111</v>
+        <v>146</v>
       </c>
       <c r="H28" t="s">
-        <v>112</v>
-      </c>
-      <c r="S28" t="s">
-        <v>113</v>
-      </c>
-      <c r="U28" t="s">
-        <v>41</v>
+        <v>147</v>
+      </c>
+      <c r="P28" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
@@ -1924,48 +1948,16 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>144</v>
+        <v>106</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>169</v>
+        <v>105</v>
       </c>
       <c r="F29" t="s">
-        <v>145</v>
+        <v>106</v>
       </c>
       <c r="G29" t="s">
-        <v>146</v>
-      </c>
-      <c r="H29" t="s">
-        <v>147</v>
-      </c>
-      <c r="P29" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>1</v>
-      </c>
-      <c r="B30" t="s">
-        <v>28</v>
-      </c>
-      <c r="F30" t="s">
-        <v>29</v>
-      </c>
-      <c r="G30" t="s">
-        <v>30</v>
-      </c>
-      <c r="H30" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
@@ -1973,13 +1965,13 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F31" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G31" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H31" t="s">
         <v>31</v>
@@ -1990,16 +1982,13 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>127</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>126</v>
+        <v>32</v>
       </c>
       <c r="F32" t="s">
-        <v>128</v>
+        <v>33</v>
       </c>
       <c r="G32" t="s">
-        <v>126</v>
+        <v>34</v>
       </c>
       <c r="H32" t="s">
         <v>31</v>
@@ -2010,16 +1999,16 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>94</v>
+        <v>127</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="F33" t="s">
-        <v>95</v>
+        <v>128</v>
       </c>
       <c r="G33" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="H33" t="s">
         <v>31</v>
@@ -2033,13 +2022,13 @@
         <v>94</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F34" t="s">
         <v>95</v>
       </c>
       <c r="G34" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H34" t="s">
         <v>31</v>
@@ -2053,13 +2042,13 @@
         <v>94</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="F35" t="s">
         <v>95</v>
       </c>
       <c r="G35" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="H35" t="s">
         <v>31</v>
@@ -2073,13 +2062,13 @@
         <v>94</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F36" t="s">
         <v>95</v>
       </c>
       <c r="G36" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H36" t="s">
         <v>31</v>
@@ -2090,16 +2079,16 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="F37" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="G37" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="H37" t="s">
         <v>31</v>
@@ -2110,18 +2099,38 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
+        <v>119</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F38" t="s">
+        <v>120</v>
+      </c>
+      <c r="G38" t="s">
+        <v>121</v>
+      </c>
+      <c r="H38" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
         <v>123</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C39" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F39" t="s">
         <v>124</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G39" t="s">
         <v>125</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H39" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2137,6 +2146,7 @@
     <hyperlink ref="E12" r:id="rId8" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP1206FTD20K0/RNCP1206FTD20K0CT-ND/2240718" xr:uid="{116631FA-D811-884C-B276-9CADAAEF69F4}"/>
     <hyperlink ref="E8" r:id="rId9" display="https://www.digikey.com/product-detail/en/te-connectivity-passive-product/CRG1206F4K7/A106078CT-ND/3477735" xr:uid="{54F5A1F9-1D87-0A40-A492-AFC72B5AAEE0}"/>
     <hyperlink ref="E4" r:id="rId10" display="https://www.digikey.com/product-detail/en/yageo/CC1206JRNPOBBN561/311-4436-1-ND/8025525" xr:uid="{39858258-CC5F-A247-B310-151D6A733093}"/>
+    <hyperlink ref="E25" r:id="rId11" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/691111710003/732-2031-ND/2060527" xr:uid="{DAB4E495-D56A-CE4B-BBBE-A993FC7D5264}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Added URL for click-jack to BoM
</commit_message>
<xml_diff>
--- a/Electronics/Low Level v3/BoM.xlsx
+++ b/Electronics/Low Level v3/BoM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Projects/elcano/Electronics/Low Level v3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B53FC5D-3B06-A245-ADBA-15DAD99665E4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9817737A-49D1-8948-890E-72CDF67D6874}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1040" windowWidth="33600" windowHeight="20560" xr2:uid="{F66CC82F-6637-7D48-A4BB-0FCD493187ED}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="21160" xr2:uid="{F66CC82F-6637-7D48-A4BB-0FCD493187ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{CC92EAD6-DDB1-3040-8FBD-65C1CB1989B6}" name="LowLevelv3" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/ben/Downloads/LowLevelv3.csv" tab="0" semicolon="1">
+    <textPr sourceFile="/Users/ben/Downloads/LowLevelv3.csv" tab="0" semicolon="1">
       <textFields count="22">
         <textField/>
         <textField/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="199">
   <si>
     <t>Qty</t>
   </si>
@@ -660,13 +660,16 @@
   </si>
   <si>
     <t>732-2031-ND</t>
+  </si>
+  <si>
+    <t>‎MJ1-2503A‎</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -696,6 +699,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0000EE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -718,7 +728,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -735,6 +745,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1056,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A12E2CF-710F-D148-A35C-437BFC6C6DF7}">
   <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="141" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1953,6 +1964,12 @@
       <c r="C29" s="4" t="s">
         <v>105</v>
       </c>
+      <c r="D29" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>198</v>
+      </c>
       <c r="F29" t="s">
         <v>106</v>
       </c>

</xml_diff>